<commit_message>
Added updated Excel workbook
I added a column for Code2000 font, and added a cell comment for Armenian Hyphen.
</commit_message>
<xml_diff>
--- a/Armenian Font Mapping Table.xlsx
+++ b/Armenian Font Mapping Table.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Unconfirmed from PDF RTF" sheetId="6" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Armenian Font Mapping Table'!$A$1:$L$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Armenian Font Mapping Table'!$A$1:$M$96</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Converted to ArmSCII-7'!$A$1:$G$92</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -92,7 +92,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Code2000 font</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +118,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="K90" authorId="0">
+    <comment ref="D89" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Armenian hyphen is not supported in Times Armenian.
+Workaround was to use \--</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L90" authorId="0">
       <text>
         <r>
           <rPr>
@@ -118,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K91" authorId="0">
+    <comment ref="L91" authorId="0">
       <text>
         <r>
           <rPr>
@@ -275,7 +302,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="597">
   <si>
     <t>\'a4</t>
   </si>
@@ -2075,7 +2102,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2292,6 +2319,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Code2000"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Code2000"/>
     </font>
   </fonts>
   <fills count="37">
@@ -2659,7 +2696,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2717,6 +2754,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3054,11 +3100,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L98"/>
+  <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3068,14 +3114,15 @@
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="33" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -3098,22 +3145,25 @@
         <v>91</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="M1" s="26" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="19.5">
+    <row r="2" spans="1:13" ht="19.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3135,25 +3185,28 @@
       <c r="G2" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="31" t="s">
+        <v>561</v>
+      </c>
+      <c r="I2" s="16" t="s">
         <v>560</v>
       </c>
-      <c r="I2" s="15">
-        <f>HEX2DEC(H2)</f>
+      <c r="J2" s="15">
+        <f t="shared" ref="J2:J33" si="0">HEX2DEC(I2)</f>
         <v>1417</v>
       </c>
-      <c r="J2" t="str">
-        <f>"\u"&amp;TEXT(I2,"0000")&amp;"?"</f>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K33" si="1">"\u"&amp;TEXT(J2,"0000")&amp;"?"</f>
         <v>\u1417?</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>559</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="M2" s="25" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="19.5">
+    <row r="3" spans="1:13" ht="19.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3167,32 +3220,35 @@
         <v>0</v>
       </c>
       <c r="E3" s="24" t="str">
-        <f>F3</f>
+        <f t="shared" ref="E3:E34" si="2">F3</f>
         <v>¤</v>
       </c>
       <c r="F3" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D3,2)))</f>
+        <f t="shared" ref="F3:F34" si="3">CHAR(HEX2DEC(RIGHT(D3,2)))</f>
         <v>¤</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="I3" s="15">
-        <f>HEX2DEC(H3)</f>
+      <c r="J3" s="15">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="J3" t="str">
-        <f>"\u"&amp;TEXT(I3,"0000")&amp;"?"</f>
+      <c r="K3" t="str">
+        <f t="shared" si="1"/>
         <v>\u0041?</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="19.5">
+    <row r="4" spans="1:13" ht="19.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3206,32 +3262,35 @@
         <v>1</v>
       </c>
       <c r="E4" s="24" t="str">
-        <f>F4</f>
+        <f t="shared" si="2"/>
         <v>¥</v>
       </c>
       <c r="F4" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D4,2)))</f>
+        <f t="shared" si="3"/>
         <v>¥</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="I4" s="15">
-        <f>HEX2DEC(H4)</f>
+      <c r="J4" s="15">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="J4" t="str">
-        <f>"\u"&amp;TEXT(I4,"0000")&amp;"?"</f>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
         <v>\u0040?</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="19.5">
+    <row r="5" spans="1:13" ht="19.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3245,35 +3304,38 @@
         <v>2</v>
       </c>
       <c r="E5" s="24" t="str">
-        <f>F5</f>
+        <f t="shared" si="2"/>
         <v>¦</v>
       </c>
       <c r="F5" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D5,2)))</f>
+        <f t="shared" si="3"/>
         <v>¦</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="I5" s="15">
-        <f>HEX2DEC(H5)</f>
+      <c r="J5" s="15">
+        <f t="shared" si="0"/>
         <v>187</v>
       </c>
-      <c r="J5" t="str">
-        <f>"\u"&amp;TEXT(I5,"0000")&amp;"?"</f>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
         <v>\u0187?</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>105</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="M5" s="25" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="19.5">
+    <row r="6" spans="1:13" ht="19.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3287,35 +3349,38 @@
         <v>3</v>
       </c>
       <c r="E6" s="24" t="str">
-        <f>F6</f>
+        <f t="shared" si="2"/>
         <v>§</v>
       </c>
       <c r="F6" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D6,2)))</f>
+        <f t="shared" si="3"/>
         <v>§</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="I6" s="15">
-        <f>HEX2DEC(H6)</f>
+      <c r="J6" s="15">
+        <f t="shared" si="0"/>
         <v>171</v>
       </c>
-      <c r="J6" t="str">
-        <f>"\u"&amp;TEXT(I6,"0000")&amp;"?"</f>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
         <v>\u0171?</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>100</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="M6" s="25" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="19.5">
+    <row r="7" spans="1:13" ht="19.5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3329,32 +3394,35 @@
         <v>4</v>
       </c>
       <c r="E7" s="24" t="str">
-        <f>F7</f>
+        <f t="shared" si="2"/>
         <v>¨</v>
       </c>
       <c r="F7" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D7,2)))</f>
+        <f t="shared" si="3"/>
         <v>¨</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="I7" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="I7" s="15">
-        <f>HEX2DEC(H7)</f>
+      <c r="J7" s="15">
+        <f t="shared" si="0"/>
         <v>1415</v>
       </c>
-      <c r="J7" t="str">
-        <f>"\u"&amp;TEXT(I7,"0000")&amp;"?"</f>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
         <v>\u1415?</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="L7" s="9" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="18.75">
+    <row r="8" spans="1:13" ht="18.75">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3368,35 +3436,38 @@
         <v>5</v>
       </c>
       <c r="E8" s="24" t="str">
-        <f>F8</f>
+        <f t="shared" si="2"/>
         <v>©</v>
       </c>
       <c r="F8" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D8,2)))</f>
+        <f t="shared" si="3"/>
         <v>©</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="33" t="s">
+        <v>572</v>
+      </c>
+      <c r="I8" s="16" t="s">
         <v>574</v>
       </c>
-      <c r="I8" s="15">
-        <f>HEX2DEC(H8)</f>
+      <c r="J8" s="15">
+        <f t="shared" si="0"/>
         <v>8228</v>
       </c>
-      <c r="J8" t="str">
-        <f>"\u"&amp;TEXT(I8,"0000")&amp;"?"</f>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
         <v>\u8228?</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="L8" s="27" t="s">
         <v>573</v>
       </c>
-      <c r="L8" s="25" t="s">
+      <c r="M8" s="25" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="19.5">
+    <row r="9" spans="1:13" ht="19.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3410,35 +3481,38 @@
         <v>6</v>
       </c>
       <c r="E9" s="24" t="str">
-        <f>F9</f>
+        <f t="shared" si="2"/>
         <v>ª</v>
       </c>
       <c r="F9" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D9,2)))</f>
+        <f t="shared" si="3"/>
         <v>ª</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="I9" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="I9" s="15">
-        <f>HEX2DEC(H9)</f>
+      <c r="J9" s="15">
+        <f t="shared" si="0"/>
         <v>1373</v>
       </c>
-      <c r="J9" t="str">
-        <f>"\u"&amp;TEXT(I9,"0000")&amp;"?"</f>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
         <v>\u1373?</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>202</v>
       </c>
-      <c r="L9" s="25" t="s">
+      <c r="M9" s="25" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="19.5">
+    <row r="10" spans="1:13" ht="19.5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3452,35 +3526,38 @@
         <v>7</v>
       </c>
       <c r="E10" s="24" t="str">
-        <f>F10</f>
+        <f t="shared" si="2"/>
         <v>¯</v>
       </c>
       <c r="F10" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D10,2)))</f>
+        <f t="shared" si="3"/>
         <v>¯</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="I10" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="I10" s="15">
-        <f>HEX2DEC(H10)</f>
+      <c r="J10" s="15">
+        <f t="shared" si="0"/>
         <v>1372</v>
       </c>
-      <c r="J10" t="str">
-        <f>"\u"&amp;TEXT(I10,"0000")&amp;"?"</f>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
         <v>\u1372?</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>199</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="M10" s="25" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="19.5">
+    <row r="11" spans="1:13" ht="19.5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3494,35 +3571,38 @@
         <v>8</v>
       </c>
       <c r="E11" s="24" t="str">
-        <f>F11</f>
+        <f t="shared" si="2"/>
         <v>°</v>
       </c>
       <c r="F11" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D11,2)))</f>
+        <f t="shared" si="3"/>
         <v>°</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="I11" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="I11" s="15">
-        <f>HEX2DEC(H11)</f>
+      <c r="J11" s="15">
+        <f t="shared" si="0"/>
         <v>1371</v>
       </c>
-      <c r="J11" t="str">
-        <f>"\u"&amp;TEXT(I11,"0000")&amp;"?"</f>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
         <v>\u1371?</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>196</v>
       </c>
-      <c r="L11" s="25" t="s">
+      <c r="M11" s="25" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="19.5">
+    <row r="12" spans="1:13" ht="19.5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3536,35 +3616,38 @@
         <v>9</v>
       </c>
       <c r="E12" s="24" t="str">
-        <f>F12</f>
+        <f t="shared" si="2"/>
         <v>±</v>
       </c>
       <c r="F12" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D12,2)))</f>
+        <f t="shared" si="3"/>
         <v>±</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="I12" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="I12" s="15">
-        <f>HEX2DEC(H12)</f>
+      <c r="J12" s="15">
+        <f t="shared" si="0"/>
         <v>1374</v>
       </c>
-      <c r="J12" t="str">
-        <f>"\u"&amp;TEXT(I12,"0000")&amp;"?"</f>
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
         <v>\u1374?</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>205</v>
       </c>
-      <c r="L12" s="25" t="s">
+      <c r="M12" s="25" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="19.5">
+    <row r="13" spans="1:13" ht="19.5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3578,32 +3661,35 @@
         <v>10</v>
       </c>
       <c r="E13" s="24" t="str">
-        <f>F13</f>
+        <f t="shared" si="2"/>
         <v>²</v>
       </c>
       <c r="F13" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D13,2)))</f>
+        <f t="shared" si="3"/>
         <v>²</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="I13" s="15">
-        <f>HEX2DEC(H13)</f>
+      <c r="J13" s="15">
+        <f t="shared" si="0"/>
         <v>1329</v>
       </c>
-      <c r="J13" t="str">
-        <f>"\u"&amp;TEXT(I13,"0000")&amp;"?"</f>
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
         <v>\u1329?</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="19.5">
+    <row r="14" spans="1:13" ht="19.5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3617,32 +3703,35 @@
         <v>11</v>
       </c>
       <c r="E14" s="24" t="str">
-        <f>F14</f>
+        <f t="shared" si="2"/>
         <v>³</v>
       </c>
       <c r="F14" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D14,2)))</f>
+        <f t="shared" si="3"/>
         <v>³</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="I14" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="I14" s="15">
-        <f>HEX2DEC(H14)</f>
+      <c r="J14" s="15">
+        <f t="shared" si="0"/>
         <v>1377</v>
       </c>
-      <c r="J14" t="str">
-        <f>"\u"&amp;TEXT(I14,"0000")&amp;"?"</f>
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
         <v>\u1377?</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="19.5">
+    <row r="15" spans="1:13" ht="19.5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3656,32 +3745,35 @@
         <v>12</v>
       </c>
       <c r="E15" s="24" t="str">
-        <f>F15</f>
+        <f t="shared" si="2"/>
         <v>´</v>
       </c>
       <c r="F15" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D15,2)))</f>
+        <f t="shared" si="3"/>
         <v>´</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="I15" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="I15" s="15">
-        <f>HEX2DEC(H15)</f>
+      <c r="J15" s="15">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
-      <c r="J15" t="str">
-        <f>"\u"&amp;TEXT(I15,"0000")&amp;"?"</f>
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
         <v>\u1330?</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="19.5">
+    <row r="16" spans="1:13" ht="19.5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3695,32 +3787,35 @@
         <v>13</v>
       </c>
       <c r="E16" s="24" t="str">
-        <f>F16</f>
+        <f t="shared" si="2"/>
         <v>µ</v>
       </c>
       <c r="F16" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D16,2)))</f>
+        <f t="shared" si="3"/>
         <v>µ</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="I16" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="I16" s="15">
-        <f>HEX2DEC(H16)</f>
+      <c r="J16" s="15">
+        <f t="shared" si="0"/>
         <v>1378</v>
       </c>
-      <c r="J16" t="str">
-        <f>"\u"&amp;TEXT(I16,"0000")&amp;"?"</f>
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
         <v>\u1378?</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="19.5">
+    <row r="17" spans="1:12" ht="19.5">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3734,32 +3829,35 @@
         <v>14</v>
       </c>
       <c r="E17" s="24" t="str">
-        <f>F17</f>
+        <f t="shared" si="2"/>
         <v>¶</v>
       </c>
       <c r="F17" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D17,2)))</f>
+        <f t="shared" si="3"/>
         <v>¶</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="I17" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="I17" s="15">
-        <f>HEX2DEC(H17)</f>
+      <c r="J17" s="15">
+        <f t="shared" si="0"/>
         <v>1331</v>
       </c>
-      <c r="J17" t="str">
-        <f>"\u"&amp;TEXT(I17,"0000")&amp;"?"</f>
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
         <v>\u1331?</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="19.5">
+    <row r="18" spans="1:12" ht="19.5">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3773,32 +3871,35 @@
         <v>15</v>
       </c>
       <c r="E18" s="24" t="str">
-        <f>F18</f>
+        <f t="shared" si="2"/>
         <v>·</v>
       </c>
       <c r="F18" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D18,2)))</f>
+        <f t="shared" si="3"/>
         <v>·</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="I18" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="I18" s="15">
-        <f>HEX2DEC(H18)</f>
+      <c r="J18" s="15">
+        <f t="shared" si="0"/>
         <v>1379</v>
       </c>
-      <c r="J18" t="str">
-        <f>"\u"&amp;TEXT(I18,"0000")&amp;"?"</f>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
         <v>\u1379?</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="19.5">
+    <row r="19" spans="1:12" ht="19.5">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3812,32 +3913,35 @@
         <v>16</v>
       </c>
       <c r="E19" s="24" t="str">
-        <f>F19</f>
+        <f t="shared" si="2"/>
         <v>¸</v>
       </c>
       <c r="F19" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D19,2)))</f>
+        <f t="shared" si="3"/>
         <v>¸</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="I19" s="16" t="s">
         <v>318</v>
       </c>
-      <c r="I19" s="15">
-        <f>HEX2DEC(H19)</f>
+      <c r="J19" s="15">
+        <f t="shared" si="0"/>
         <v>1332</v>
       </c>
-      <c r="J19" t="str">
-        <f>"\u"&amp;TEXT(I19,"0000")&amp;"?"</f>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
         <v>\u1332?</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="19.5">
+    <row r="20" spans="1:12" ht="19.5">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3851,32 +3955,35 @@
         <v>17</v>
       </c>
       <c r="E20" s="24" t="str">
-        <f>F20</f>
+        <f t="shared" si="2"/>
         <v>¹</v>
       </c>
       <c r="F20" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D20,2)))</f>
+        <f t="shared" si="3"/>
         <v>¹</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="I20" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="I20" s="15">
-        <f>HEX2DEC(H20)</f>
+      <c r="J20" s="15">
+        <f t="shared" si="0"/>
         <v>1380</v>
       </c>
-      <c r="J20" t="str">
-        <f>"\u"&amp;TEXT(I20,"0000")&amp;"?"</f>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
         <v>\u1380?</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="19.5">
+    <row r="21" spans="1:12" ht="19.5">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3890,32 +3997,35 @@
         <v>18</v>
       </c>
       <c r="E21" s="24" t="str">
-        <f>F21</f>
+        <f t="shared" si="2"/>
         <v>º</v>
       </c>
       <c r="F21" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D21,2)))</f>
+        <f t="shared" si="3"/>
         <v>º</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="I21" s="15">
-        <f>HEX2DEC(H21)</f>
+      <c r="J21" s="15">
+        <f t="shared" si="0"/>
         <v>1333</v>
       </c>
-      <c r="J21" t="str">
-        <f>"\u"&amp;TEXT(I21,"0000")&amp;"?"</f>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
         <v>\u1333?</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="19.5">
+    <row r="22" spans="1:12" ht="19.5">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3929,32 +4039,35 @@
         <v>19</v>
       </c>
       <c r="E22" s="24" t="str">
-        <f>F22</f>
+        <f t="shared" si="2"/>
         <v>»</v>
       </c>
       <c r="F22" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D22,2)))</f>
+        <f t="shared" si="3"/>
         <v>»</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H22" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="I22" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="I22" s="15">
-        <f>HEX2DEC(H22)</f>
+      <c r="J22" s="15">
+        <f t="shared" si="0"/>
         <v>1381</v>
       </c>
-      <c r="J22" t="str">
-        <f>"\u"&amp;TEXT(I22,"0000")&amp;"?"</f>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
         <v>\u1381?</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="19.5">
+    <row r="23" spans="1:12" ht="19.5">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3968,32 +4081,35 @@
         <v>20</v>
       </c>
       <c r="E23" s="24" t="str">
-        <f>F23</f>
+        <f t="shared" si="2"/>
         <v>¼</v>
       </c>
       <c r="F23" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D23,2)))</f>
+        <f t="shared" si="3"/>
         <v>¼</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H23" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="I23" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="I23" s="15">
-        <f>HEX2DEC(H23)</f>
+      <c r="J23" s="15">
+        <f t="shared" si="0"/>
         <v>1334</v>
       </c>
-      <c r="J23" t="str">
-        <f>"\u"&amp;TEXT(I23,"0000")&amp;"?"</f>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
         <v>\u1334?</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="19.5">
+    <row r="24" spans="1:12" ht="19.5">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4007,32 +4123,35 @@
         <v>21</v>
       </c>
       <c r="E24" s="24" t="str">
-        <f>F24</f>
+        <f t="shared" si="2"/>
         <v>½</v>
       </c>
       <c r="F24" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D24,2)))</f>
+        <f t="shared" si="3"/>
         <v>½</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H24" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="I24" s="16" t="s">
         <v>323</v>
       </c>
-      <c r="I24" s="15">
-        <f>HEX2DEC(H24)</f>
+      <c r="J24" s="15">
+        <f t="shared" si="0"/>
         <v>1382</v>
       </c>
-      <c r="J24" t="str">
-        <f>"\u"&amp;TEXT(I24,"0000")&amp;"?"</f>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
         <v>\u1382?</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="19.5">
+    <row r="25" spans="1:12" ht="19.5">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4046,32 +4165,35 @@
         <v>22</v>
       </c>
       <c r="E25" s="24" t="str">
-        <f>F25</f>
+        <f t="shared" si="2"/>
         <v>¾</v>
       </c>
       <c r="F25" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D25,2)))</f>
+        <f t="shared" si="3"/>
         <v>¾</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H25" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="I25" s="16" t="s">
         <v>324</v>
       </c>
-      <c r="I25" s="15">
-        <f>HEX2DEC(H25)</f>
+      <c r="J25" s="15">
+        <f t="shared" si="0"/>
         <v>1335</v>
       </c>
-      <c r="J25" t="str">
-        <f>"\u"&amp;TEXT(I25,"0000")&amp;"?"</f>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
         <v>\u1335?</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="19.5">
+    <row r="26" spans="1:12" ht="19.5">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4085,32 +4207,35 @@
         <v>23</v>
       </c>
       <c r="E26" s="24" t="str">
-        <f>F26</f>
+        <f t="shared" si="2"/>
         <v>¿</v>
       </c>
       <c r="F26" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D26,2)))</f>
+        <f t="shared" si="3"/>
         <v>¿</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H26" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="I26" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="I26" s="15">
-        <f>HEX2DEC(H26)</f>
+      <c r="J26" s="15">
+        <f t="shared" si="0"/>
         <v>1383</v>
       </c>
-      <c r="J26" t="str">
-        <f>"\u"&amp;TEXT(I26,"0000")&amp;"?"</f>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
         <v>\u1383?</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="19.5">
+    <row r="27" spans="1:12" ht="19.5">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4124,32 +4249,35 @@
         <v>24</v>
       </c>
       <c r="E27" s="24" t="str">
-        <f>F27</f>
+        <f t="shared" si="2"/>
         <v>À</v>
       </c>
       <c r="F27" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D27,2)))</f>
+        <f t="shared" si="3"/>
         <v>À</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="I27" s="16" t="s">
         <v>326</v>
       </c>
-      <c r="I27" s="15">
-        <f>HEX2DEC(H27)</f>
+      <c r="J27" s="15">
+        <f t="shared" si="0"/>
         <v>1336</v>
       </c>
-      <c r="J27" t="str">
-        <f>"\u"&amp;TEXT(I27,"0000")&amp;"?"</f>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
         <v>\u1336?</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="19.5">
+    <row r="28" spans="1:12" ht="19.5">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4163,32 +4291,35 @@
         <v>25</v>
       </c>
       <c r="E28" s="24" t="str">
-        <f>F28</f>
+        <f t="shared" si="2"/>
         <v>Á</v>
       </c>
       <c r="F28" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D28,2)))</f>
+        <f t="shared" si="3"/>
         <v>Á</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="H28" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="I28" s="16" t="s">
         <v>327</v>
       </c>
-      <c r="I28" s="15">
-        <f>HEX2DEC(H28)</f>
+      <c r="J28" s="15">
+        <f t="shared" si="0"/>
         <v>1384</v>
       </c>
-      <c r="J28" t="str">
-        <f>"\u"&amp;TEXT(I28,"0000")&amp;"?"</f>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
         <v>\u1384?</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="19.5">
+    <row r="29" spans="1:12" ht="19.5">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4202,32 +4333,35 @@
         <v>26</v>
       </c>
       <c r="E29" s="24" t="str">
-        <f>F29</f>
+        <f t="shared" si="2"/>
         <v>Â</v>
       </c>
       <c r="F29" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D29,2)))</f>
+        <f t="shared" si="3"/>
         <v>Â</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="H29" s="16" t="s">
+      <c r="H29" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="I29" s="16" t="s">
         <v>328</v>
       </c>
-      <c r="I29" s="15">
-        <f>HEX2DEC(H29)</f>
+      <c r="J29" s="15">
+        <f t="shared" si="0"/>
         <v>1337</v>
       </c>
-      <c r="J29" t="str">
-        <f>"\u"&amp;TEXT(I29,"0000")&amp;"?"</f>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
         <v>\u1337?</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="19.5">
+    <row r="30" spans="1:12" ht="19.5">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4241,32 +4375,35 @@
         <v>27</v>
       </c>
       <c r="E30" s="24" t="str">
-        <f>F30</f>
+        <f t="shared" si="2"/>
         <v>Ã</v>
       </c>
       <c r="F30" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D30,2)))</f>
+        <f t="shared" si="3"/>
         <v>Ã</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="H30" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="I30" s="16" t="s">
         <v>329</v>
       </c>
-      <c r="I30" s="15">
-        <f>HEX2DEC(H30)</f>
+      <c r="J30" s="15">
+        <f t="shared" si="0"/>
         <v>1385</v>
       </c>
-      <c r="J30" t="str">
-        <f>"\u"&amp;TEXT(I30,"0000")&amp;"?"</f>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
         <v>\u1385?</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="19.5">
+    <row r="31" spans="1:12" ht="19.5">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4280,32 +4417,35 @@
         <v>28</v>
       </c>
       <c r="E31" s="24" t="str">
-        <f>F31</f>
+        <f t="shared" si="2"/>
         <v>Ä</v>
       </c>
       <c r="F31" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D31,2)))</f>
+        <f t="shared" si="3"/>
         <v>Ä</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H31" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="I31" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="I31" s="15">
-        <f>HEX2DEC(H31)</f>
+      <c r="J31" s="15">
+        <f t="shared" si="0"/>
         <v>1338</v>
       </c>
-      <c r="J31" t="str">
-        <f>"\u"&amp;TEXT(I31,"0000")&amp;"?"</f>
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
         <v>\u1338?</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="19.5">
+    <row r="32" spans="1:12" ht="19.5">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4319,32 +4459,35 @@
         <v>29</v>
       </c>
       <c r="E32" s="24" t="str">
-        <f>F32</f>
+        <f t="shared" si="2"/>
         <v>Å</v>
       </c>
       <c r="F32" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D32,2)))</f>
+        <f t="shared" si="3"/>
         <v>Å</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H32" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="I32" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="I32" s="15">
-        <f>HEX2DEC(H32)</f>
+      <c r="J32" s="15">
+        <f t="shared" si="0"/>
         <v>1386</v>
       </c>
-      <c r="J32" t="str">
-        <f>"\u"&amp;TEXT(I32,"0000")&amp;"?"</f>
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
         <v>\u1386?</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="19.5">
+    <row r="33" spans="1:12" ht="19.5">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4358,32 +4501,35 @@
         <v>30</v>
       </c>
       <c r="E33" s="24" t="str">
-        <f>F33</f>
+        <f t="shared" si="2"/>
         <v>Æ</v>
       </c>
       <c r="F33" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D33,2)))</f>
+        <f t="shared" si="3"/>
         <v>Æ</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H33" s="16" t="s">
+      <c r="H33" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="I33" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="I33" s="15">
-        <f>HEX2DEC(H33)</f>
+      <c r="J33" s="15">
+        <f t="shared" si="0"/>
         <v>1339</v>
       </c>
-      <c r="J33" t="str">
-        <f>"\u"&amp;TEXT(I33,"0000")&amp;"?"</f>
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
         <v>\u1339?</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="19.5">
+    <row r="34" spans="1:12" ht="19.5">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4397,32 +4543,35 @@
         <v>31</v>
       </c>
       <c r="E34" s="24" t="str">
-        <f>F34</f>
+        <f t="shared" si="2"/>
         <v>Ç</v>
       </c>
       <c r="F34" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D34,2)))</f>
+        <f t="shared" si="3"/>
         <v>Ç</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="H34" s="16" t="s">
+      <c r="H34" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="I34" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="I34" s="15">
-        <f>HEX2DEC(H34)</f>
+      <c r="J34" s="15">
+        <f t="shared" ref="J34:J65" si="4">HEX2DEC(I34)</f>
         <v>1387</v>
       </c>
-      <c r="J34" t="str">
-        <f>"\u"&amp;TEXT(I34,"0000")&amp;"?"</f>
+      <c r="K34" t="str">
+        <f t="shared" ref="K34:K65" si="5">"\u"&amp;TEXT(J34,"0000")&amp;"?"</f>
         <v>\u1387?</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="19.5">
+    <row r="35" spans="1:12" ht="19.5">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4436,32 +4585,35 @@
         <v>32</v>
       </c>
       <c r="E35" s="24" t="str">
-        <f>F35</f>
+        <f t="shared" ref="E35:E66" si="6">F35</f>
         <v>È</v>
       </c>
       <c r="F35" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D35,2)))</f>
+        <f t="shared" ref="F35:F66" si="7">CHAR(HEX2DEC(RIGHT(D35,2)))</f>
         <v>È</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="H35" s="16" t="s">
+      <c r="H35" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="I35" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="I35" s="15">
-        <f>HEX2DEC(H35)</f>
+      <c r="J35" s="15">
+        <f t="shared" si="4"/>
         <v>1340</v>
       </c>
-      <c r="J35" t="str">
-        <f>"\u"&amp;TEXT(I35,"0000")&amp;"?"</f>
+      <c r="K35" t="str">
+        <f t="shared" si="5"/>
         <v>\u1340?</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="19.5">
+    <row r="36" spans="1:12" ht="19.5">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4475,32 +4627,35 @@
         <v>33</v>
       </c>
       <c r="E36" s="24" t="str">
-        <f>F36</f>
+        <f t="shared" si="6"/>
         <v>É</v>
       </c>
       <c r="F36" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D36,2)))</f>
+        <f t="shared" si="7"/>
         <v>É</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="H36" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="I36" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="I36" s="15">
-        <f>HEX2DEC(H36)</f>
+      <c r="J36" s="15">
+        <f t="shared" si="4"/>
         <v>1388</v>
       </c>
-      <c r="J36" t="str">
-        <f>"\u"&amp;TEXT(I36,"0000")&amp;"?"</f>
+      <c r="K36" t="str">
+        <f t="shared" si="5"/>
         <v>\u1388?</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="19.5">
+    <row r="37" spans="1:12" ht="19.5">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4514,32 +4669,35 @@
         <v>34</v>
       </c>
       <c r="E37" s="24" t="str">
-        <f>F37</f>
+        <f t="shared" si="6"/>
         <v>Ê</v>
       </c>
       <c r="F37" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D37,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ê</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="H37" s="16" t="s">
+      <c r="H37" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="I37" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="I37" s="15">
-        <f>HEX2DEC(H37)</f>
+      <c r="J37" s="15">
+        <f t="shared" si="4"/>
         <v>1341</v>
       </c>
-      <c r="J37" t="str">
-        <f>"\u"&amp;TEXT(I37,"0000")&amp;"?"</f>
+      <c r="K37" t="str">
+        <f t="shared" si="5"/>
         <v>\u1341?</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="19.5">
+    <row r="38" spans="1:12" ht="19.5">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4553,32 +4711,35 @@
         <v>35</v>
       </c>
       <c r="E38" s="24" t="str">
-        <f>F38</f>
+        <f t="shared" si="6"/>
         <v>Ë</v>
       </c>
       <c r="F38" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D38,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ë</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="H38" s="16" t="s">
+      <c r="H38" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="I38" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="I38" s="15">
-        <f>HEX2DEC(H38)</f>
+      <c r="J38" s="15">
+        <f t="shared" si="4"/>
         <v>1389</v>
       </c>
-      <c r="J38" t="str">
-        <f>"\u"&amp;TEXT(I38,"0000")&amp;"?"</f>
+      <c r="K38" t="str">
+        <f t="shared" si="5"/>
         <v>\u1389?</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="19.5">
+    <row r="39" spans="1:12" ht="19.5">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4592,32 +4753,35 @@
         <v>36</v>
       </c>
       <c r="E39" s="24" t="str">
-        <f>F39</f>
+        <f t="shared" si="6"/>
         <v>Ì</v>
       </c>
       <c r="F39" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D39,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ì</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H39" s="16" t="s">
+      <c r="H39" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="I39" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="I39" s="15">
-        <f>HEX2DEC(H39)</f>
+      <c r="J39" s="15">
+        <f t="shared" si="4"/>
         <v>1342</v>
       </c>
-      <c r="J39" t="str">
-        <f>"\u"&amp;TEXT(I39,"0000")&amp;"?"</f>
+      <c r="K39" t="str">
+        <f t="shared" si="5"/>
         <v>\u1342?</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="19.5">
+    <row r="40" spans="1:12" ht="19.5">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4631,32 +4795,35 @@
         <v>37</v>
       </c>
       <c r="E40" s="24" t="str">
-        <f>F40</f>
+        <f t="shared" si="6"/>
         <v>Í</v>
       </c>
       <c r="F40" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D40,2)))</f>
+        <f t="shared" si="7"/>
         <v>Í</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="H40" s="16" t="s">
+      <c r="H40" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="I40" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="I40" s="15">
-        <f>HEX2DEC(H40)</f>
+      <c r="J40" s="15">
+        <f t="shared" si="4"/>
         <v>1390</v>
       </c>
-      <c r="J40" t="str">
-        <f>"\u"&amp;TEXT(I40,"0000")&amp;"?"</f>
+      <c r="K40" t="str">
+        <f t="shared" si="5"/>
         <v>\u1390?</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="19.5">
+    <row r="41" spans="1:12" ht="19.5">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4670,32 +4837,35 @@
         <v>38</v>
       </c>
       <c r="E41" s="24" t="str">
-        <f>F41</f>
+        <f t="shared" si="6"/>
         <v>Î</v>
       </c>
       <c r="F41" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D41,2)))</f>
+        <f t="shared" si="7"/>
         <v>Î</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H41" s="16" t="s">
+      <c r="H41" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="I41" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="I41" s="15">
-        <f>HEX2DEC(H41)</f>
+      <c r="J41" s="15">
+        <f t="shared" si="4"/>
         <v>1343</v>
       </c>
-      <c r="J41" t="str">
-        <f>"\u"&amp;TEXT(I41,"0000")&amp;"?"</f>
+      <c r="K41" t="str">
+        <f t="shared" si="5"/>
         <v>\u1343?</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="19.5">
+    <row r="42" spans="1:12" ht="19.5">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4709,32 +4879,35 @@
         <v>39</v>
       </c>
       <c r="E42" s="24" t="str">
-        <f>F42</f>
+        <f t="shared" si="6"/>
         <v>Ï</v>
       </c>
       <c r="F42" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D42,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ï</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H42" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="I42" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="I42" s="15">
-        <f>HEX2DEC(H42)</f>
+      <c r="J42" s="15">
+        <f t="shared" si="4"/>
         <v>1391</v>
       </c>
-      <c r="J42" t="str">
-        <f>"\u"&amp;TEXT(I42,"0000")&amp;"?"</f>
+      <c r="K42" t="str">
+        <f t="shared" si="5"/>
         <v>\u1391?</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="19.5">
+    <row r="43" spans="1:12" ht="19.5">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4748,32 +4921,35 @@
         <v>40</v>
       </c>
       <c r="E43" s="24" t="str">
-        <f>F43</f>
+        <f t="shared" si="6"/>
         <v>Ð</v>
       </c>
       <c r="F43" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D43,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ð</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="H43" s="16" t="s">
+      <c r="H43" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="I43" s="16" t="s">
         <v>330</v>
       </c>
-      <c r="I43" s="15">
-        <f>HEX2DEC(H43)</f>
+      <c r="J43" s="15">
+        <f t="shared" si="4"/>
         <v>1344</v>
       </c>
-      <c r="J43" t="str">
-        <f>"\u"&amp;TEXT(I43,"0000")&amp;"?"</f>
+      <c r="K43" t="str">
+        <f t="shared" si="5"/>
         <v>\u1344?</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="19.5">
+    <row r="44" spans="1:12" ht="19.5">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4787,32 +4963,35 @@
         <v>41</v>
       </c>
       <c r="E44" s="24" t="str">
-        <f>F44</f>
+        <f t="shared" si="6"/>
         <v>Ñ</v>
       </c>
       <c r="F44" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D44,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ñ</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="H44" s="16" t="s">
+      <c r="H44" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="I44" s="16" t="s">
         <v>331</v>
       </c>
-      <c r="I44" s="15">
-        <f>HEX2DEC(H44)</f>
+      <c r="J44" s="15">
+        <f t="shared" si="4"/>
         <v>1392</v>
       </c>
-      <c r="J44" t="str">
-        <f>"\u"&amp;TEXT(I44,"0000")&amp;"?"</f>
+      <c r="K44" t="str">
+        <f t="shared" si="5"/>
         <v>\u1392?</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="19.5">
+    <row r="45" spans="1:12" ht="19.5">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4826,32 +5005,35 @@
         <v>42</v>
       </c>
       <c r="E45" s="24" t="str">
-        <f>F45</f>
+        <f t="shared" si="6"/>
         <v>Ò</v>
       </c>
       <c r="F45" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D45,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ò</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H45" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="I45" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="I45" s="15">
-        <f>HEX2DEC(H45)</f>
+      <c r="J45" s="15">
+        <f t="shared" si="4"/>
         <v>1345</v>
       </c>
-      <c r="J45" t="str">
-        <f>"\u"&amp;TEXT(I45,"0000")&amp;"?"</f>
+      <c r="K45" t="str">
+        <f t="shared" si="5"/>
         <v>\u1345?</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="19.5">
+    <row r="46" spans="1:12" ht="19.5">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4865,32 +5047,35 @@
         <v>43</v>
       </c>
       <c r="E46" s="24" t="str">
-        <f>F46</f>
+        <f t="shared" si="6"/>
         <v>Ó</v>
       </c>
       <c r="F46" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D46,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ó</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="H46" s="16" t="s">
+      <c r="H46" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="I46" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="I46" s="15">
-        <f>HEX2DEC(H46)</f>
+      <c r="J46" s="15">
+        <f t="shared" si="4"/>
         <v>1393</v>
       </c>
-      <c r="J46" t="str">
-        <f>"\u"&amp;TEXT(I46,"0000")&amp;"?"</f>
+      <c r="K46" t="str">
+        <f t="shared" si="5"/>
         <v>\u1393?</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="19.5">
+    <row r="47" spans="1:12" ht="19.5">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4904,32 +5089,35 @@
         <v>44</v>
       </c>
       <c r="E47" s="24" t="str">
-        <f>F47</f>
+        <f t="shared" si="6"/>
         <v>Ô</v>
       </c>
       <c r="F47" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D47,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ô</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="H47" s="16" t="s">
+      <c r="H47" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="I47" s="16" t="s">
         <v>334</v>
       </c>
-      <c r="I47" s="15">
-        <f>HEX2DEC(H47)</f>
+      <c r="J47" s="15">
+        <f t="shared" si="4"/>
         <v>1346</v>
       </c>
-      <c r="J47" t="str">
-        <f>"\u"&amp;TEXT(I47,"0000")&amp;"?"</f>
+      <c r="K47" t="str">
+        <f t="shared" si="5"/>
         <v>\u1346?</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="19.5">
+    <row r="48" spans="1:12" ht="19.5">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4943,32 +5131,35 @@
         <v>45</v>
       </c>
       <c r="E48" s="24" t="str">
-        <f>F48</f>
+        <f t="shared" si="6"/>
         <v>Õ</v>
       </c>
       <c r="F48" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D48,2)))</f>
+        <f t="shared" si="7"/>
         <v>Õ</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="H48" s="16" t="s">
+      <c r="H48" s="31" t="s">
+        <v>246</v>
+      </c>
+      <c r="I48" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="I48" s="15">
-        <f>HEX2DEC(H48)</f>
+      <c r="J48" s="15">
+        <f t="shared" si="4"/>
         <v>1394</v>
       </c>
-      <c r="J48" t="str">
-        <f>"\u"&amp;TEXT(I48,"0000")&amp;"?"</f>
+      <c r="K48" t="str">
+        <f t="shared" si="5"/>
         <v>\u1394?</v>
       </c>
-      <c r="K48" t="s">
+      <c r="L48" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="19.5">
+    <row r="49" spans="1:12" ht="19.5">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4982,32 +5173,35 @@
         <v>46</v>
       </c>
       <c r="E49" s="24" t="str">
-        <f>F49</f>
+        <f t="shared" si="6"/>
         <v>Ö</v>
       </c>
       <c r="F49" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D49,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ö</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="H49" s="16" t="s">
+      <c r="H49" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="I49" s="16" t="s">
         <v>336</v>
       </c>
-      <c r="I49" s="15">
-        <f>HEX2DEC(H49)</f>
+      <c r="J49" s="15">
+        <f t="shared" si="4"/>
         <v>1347</v>
       </c>
-      <c r="J49" t="str">
-        <f>"\u"&amp;TEXT(I49,"0000")&amp;"?"</f>
+      <c r="K49" t="str">
+        <f t="shared" si="5"/>
         <v>\u1347?</v>
       </c>
-      <c r="K49" t="s">
+      <c r="L49" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="19.5">
+    <row r="50" spans="1:12" ht="19.5">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5021,32 +5215,35 @@
         <v>47</v>
       </c>
       <c r="E50" s="24" t="str">
-        <f>F50</f>
+        <f t="shared" si="6"/>
         <v>×</v>
       </c>
       <c r="F50" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D50,2)))</f>
+        <f t="shared" si="7"/>
         <v>×</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="H50" s="16" t="s">
+      <c r="H50" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="I50" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="I50" s="15">
-        <f>HEX2DEC(H50)</f>
+      <c r="J50" s="15">
+        <f t="shared" si="4"/>
         <v>1395</v>
       </c>
-      <c r="J50" t="str">
-        <f>"\u"&amp;TEXT(I50,"0000")&amp;"?"</f>
+      <c r="K50" t="str">
+        <f t="shared" si="5"/>
         <v>\u1395?</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="19.5">
+    <row r="51" spans="1:12" ht="19.5">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5060,32 +5257,35 @@
         <v>48</v>
       </c>
       <c r="E51" s="24" t="str">
-        <f>F51</f>
+        <f t="shared" si="6"/>
         <v>Ø</v>
       </c>
       <c r="F51" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D51,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ø</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="H51" s="16" t="s">
+      <c r="H51" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="I51" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="I51" s="15">
-        <f>HEX2DEC(H51)</f>
+      <c r="J51" s="15">
+        <f t="shared" si="4"/>
         <v>1348</v>
       </c>
-      <c r="J51" t="str">
-        <f>"\u"&amp;TEXT(I51,"0000")&amp;"?"</f>
+      <c r="K51" t="str">
+        <f t="shared" si="5"/>
         <v>\u1348?</v>
       </c>
-      <c r="K51" t="s">
+      <c r="L51" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="19.5">
+    <row r="52" spans="1:12" ht="19.5">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5099,32 +5299,35 @@
         <v>49</v>
       </c>
       <c r="E52" s="24" t="str">
-        <f>F52</f>
+        <f t="shared" si="6"/>
         <v>Ù</v>
       </c>
       <c r="F52" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D52,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ù</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="H52" s="16" t="s">
+      <c r="H52" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="I52" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="I52" s="15">
-        <f>HEX2DEC(H52)</f>
+      <c r="J52" s="15">
+        <f t="shared" si="4"/>
         <v>1396</v>
       </c>
-      <c r="J52" t="str">
-        <f>"\u"&amp;TEXT(I52,"0000")&amp;"?"</f>
+      <c r="K52" t="str">
+        <f t="shared" si="5"/>
         <v>\u1396?</v>
       </c>
-      <c r="K52" t="s">
+      <c r="L52" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="19.5">
+    <row r="53" spans="1:12" ht="19.5">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5138,32 +5341,35 @@
         <v>50</v>
       </c>
       <c r="E53" s="24" t="str">
-        <f>F53</f>
+        <f t="shared" si="6"/>
         <v>Ú</v>
       </c>
       <c r="F53" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D53,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ú</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="H53" s="16" t="s">
+      <c r="H53" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="I53" s="16" t="s">
         <v>340</v>
       </c>
-      <c r="I53" s="15">
-        <f>HEX2DEC(H53)</f>
+      <c r="J53" s="15">
+        <f t="shared" si="4"/>
         <v>1349</v>
       </c>
-      <c r="J53" t="str">
-        <f>"\u"&amp;TEXT(I53,"0000")&amp;"?"</f>
+      <c r="K53" t="str">
+        <f t="shared" si="5"/>
         <v>\u1349?</v>
       </c>
-      <c r="K53" t="s">
+      <c r="L53" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="19.5">
+    <row r="54" spans="1:12" ht="19.5">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5177,32 +5383,35 @@
         <v>51</v>
       </c>
       <c r="E54" s="24" t="str">
-        <f>F54</f>
+        <f t="shared" si="6"/>
         <v>Û</v>
       </c>
       <c r="F54" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D54,2)))</f>
+        <f t="shared" si="7"/>
         <v>Û</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="H54" s="16" t="s">
+      <c r="H54" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="I54" s="16" t="s">
         <v>341</v>
       </c>
-      <c r="I54" s="15">
-        <f>HEX2DEC(H54)</f>
+      <c r="J54" s="15">
+        <f t="shared" si="4"/>
         <v>1397</v>
       </c>
-      <c r="J54" t="str">
-        <f>"\u"&amp;TEXT(I54,"0000")&amp;"?"</f>
+      <c r="K54" t="str">
+        <f t="shared" si="5"/>
         <v>\u1397?</v>
       </c>
-      <c r="K54" t="s">
+      <c r="L54" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="19.5">
+    <row r="55" spans="1:12" ht="19.5">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5216,32 +5425,35 @@
         <v>52</v>
       </c>
       <c r="E55" s="24" t="str">
-        <f>F55</f>
+        <f t="shared" si="6"/>
         <v>Ü</v>
       </c>
       <c r="F55" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D55,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ü</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="H55" s="16" t="s">
+      <c r="H55" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="I55" s="16" t="s">
         <v>342</v>
       </c>
-      <c r="I55" s="15">
-        <f>HEX2DEC(H55)</f>
+      <c r="J55" s="15">
+        <f t="shared" si="4"/>
         <v>1350</v>
       </c>
-      <c r="J55" t="str">
-        <f>"\u"&amp;TEXT(I55,"0000")&amp;"?"</f>
+      <c r="K55" t="str">
+        <f t="shared" si="5"/>
         <v>\u1350?</v>
       </c>
-      <c r="K55" t="s">
+      <c r="L55" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="19.5">
+    <row r="56" spans="1:12" ht="19.5">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5255,32 +5467,35 @@
         <v>53</v>
       </c>
       <c r="E56" s="24" t="str">
-        <f>F56</f>
+        <f t="shared" si="6"/>
         <v>Ý</v>
       </c>
       <c r="F56" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D56,2)))</f>
+        <f t="shared" si="7"/>
         <v>Ý</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="H56" s="16" t="s">
+      <c r="H56" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="I56" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="I56" s="15">
-        <f>HEX2DEC(H56)</f>
+      <c r="J56" s="15">
+        <f t="shared" si="4"/>
         <v>1398</v>
       </c>
-      <c r="J56" t="str">
-        <f>"\u"&amp;TEXT(I56,"0000")&amp;"?"</f>
+      <c r="K56" t="str">
+        <f t="shared" si="5"/>
         <v>\u1398?</v>
       </c>
-      <c r="K56" t="s">
+      <c r="L56" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="19.5">
+    <row r="57" spans="1:12" ht="19.5">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5294,32 +5509,35 @@
         <v>54</v>
       </c>
       <c r="E57" s="24" t="str">
-        <f>F57</f>
+        <f t="shared" si="6"/>
         <v>Þ</v>
       </c>
       <c r="F57" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D57,2)))</f>
+        <f t="shared" si="7"/>
         <v>Þ</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="H57" s="16" t="s">
+      <c r="H57" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="I57" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="I57" s="15">
-        <f>HEX2DEC(H57)</f>
+      <c r="J57" s="15">
+        <f t="shared" si="4"/>
         <v>1351</v>
       </c>
-      <c r="J57" t="str">
-        <f>"\u"&amp;TEXT(I57,"0000")&amp;"?"</f>
+      <c r="K57" t="str">
+        <f t="shared" si="5"/>
         <v>\u1351?</v>
       </c>
-      <c r="K57" t="s">
+      <c r="L57" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="19.5">
+    <row r="58" spans="1:12" ht="19.5">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5333,32 +5551,35 @@
         <v>55</v>
       </c>
       <c r="E58" s="24" t="str">
-        <f>F58</f>
+        <f t="shared" si="6"/>
         <v>ß</v>
       </c>
       <c r="F58" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D58,2)))</f>
+        <f t="shared" si="7"/>
         <v>ß</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="H58" s="16" t="s">
+      <c r="H58" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="I58" s="16" t="s">
         <v>345</v>
       </c>
-      <c r="I58" s="15">
-        <f>HEX2DEC(H58)</f>
+      <c r="J58" s="15">
+        <f t="shared" si="4"/>
         <v>1399</v>
       </c>
-      <c r="J58" t="str">
-        <f>"\u"&amp;TEXT(I58,"0000")&amp;"?"</f>
+      <c r="K58" t="str">
+        <f t="shared" si="5"/>
         <v>\u1399?</v>
       </c>
-      <c r="K58" t="s">
+      <c r="L58" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="19.5">
+    <row r="59" spans="1:12" ht="19.5">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5372,32 +5593,35 @@
         <v>56</v>
       </c>
       <c r="E59" s="24" t="str">
-        <f>F59</f>
+        <f t="shared" si="6"/>
         <v>à</v>
       </c>
       <c r="F59" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D59,2)))</f>
+        <f t="shared" si="7"/>
         <v>à</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="H59" s="16" t="s">
+      <c r="H59" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="I59" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="I59" s="15">
-        <f>HEX2DEC(H59)</f>
+      <c r="J59" s="15">
+        <f t="shared" si="4"/>
         <v>1352</v>
       </c>
-      <c r="J59" t="str">
-        <f>"\u"&amp;TEXT(I59,"0000")&amp;"?"</f>
+      <c r="K59" t="str">
+        <f t="shared" si="5"/>
         <v>\u1352?</v>
       </c>
-      <c r="K59" t="s">
+      <c r="L59" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="19.5">
+    <row r="60" spans="1:12" ht="19.5">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5411,32 +5635,35 @@
         <v>57</v>
       </c>
       <c r="E60" s="24" t="str">
-        <f>F60</f>
+        <f t="shared" si="6"/>
         <v>á</v>
       </c>
       <c r="F60" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D60,2)))</f>
+        <f t="shared" si="7"/>
         <v>á</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="H60" s="16" t="s">
+      <c r="H60" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="I60" s="16" t="s">
         <v>347</v>
       </c>
-      <c r="I60" s="15">
-        <f>HEX2DEC(H60)</f>
+      <c r="J60" s="15">
+        <f t="shared" si="4"/>
         <v>1400</v>
       </c>
-      <c r="J60" t="str">
-        <f>"\u"&amp;TEXT(I60,"0000")&amp;"?"</f>
+      <c r="K60" t="str">
+        <f t="shared" si="5"/>
         <v>\u1400?</v>
       </c>
-      <c r="K60" t="s">
+      <c r="L60" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="19.5">
+    <row r="61" spans="1:12" ht="19.5">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5450,32 +5677,35 @@
         <v>58</v>
       </c>
       <c r="E61" s="24" t="str">
-        <f>F61</f>
+        <f t="shared" si="6"/>
         <v>â</v>
       </c>
       <c r="F61" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D61,2)))</f>
+        <f t="shared" si="7"/>
         <v>â</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="H61" s="16" t="s">
+      <c r="H61" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="I61" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="I61" s="15">
-        <f>HEX2DEC(H61)</f>
+      <c r="J61" s="15">
+        <f t="shared" si="4"/>
         <v>1353</v>
       </c>
-      <c r="J61" t="str">
-        <f>"\u"&amp;TEXT(I61,"0000")&amp;"?"</f>
+      <c r="K61" t="str">
+        <f t="shared" si="5"/>
         <v>\u1353?</v>
       </c>
-      <c r="K61" t="s">
+      <c r="L61" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="19.5">
+    <row r="62" spans="1:12" ht="19.5">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5489,32 +5719,35 @@
         <v>59</v>
       </c>
       <c r="E62" s="24" t="str">
-        <f>F62</f>
+        <f t="shared" si="6"/>
         <v>ã</v>
       </c>
       <c r="F62" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D62,2)))</f>
+        <f t="shared" si="7"/>
         <v>ã</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="H62" s="16" t="s">
+      <c r="H62" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="I62" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="I62" s="15">
-        <f>HEX2DEC(H62)</f>
+      <c r="J62" s="15">
+        <f t="shared" si="4"/>
         <v>1401</v>
       </c>
-      <c r="J62" t="str">
-        <f>"\u"&amp;TEXT(I62,"0000")&amp;"?"</f>
+      <c r="K62" t="str">
+        <f t="shared" si="5"/>
         <v>\u1401?</v>
       </c>
-      <c r="K62" t="s">
+      <c r="L62" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="19.5">
+    <row r="63" spans="1:12" ht="19.5">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5528,32 +5761,35 @@
         <v>60</v>
       </c>
       <c r="E63" s="24" t="str">
-        <f>F63</f>
+        <f t="shared" si="6"/>
         <v>ä</v>
       </c>
       <c r="F63" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D63,2)))</f>
+        <f t="shared" si="7"/>
         <v>ä</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="H63" s="16" t="s">
+      <c r="H63" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="I63" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="I63" s="15">
-        <f>HEX2DEC(H63)</f>
+      <c r="J63" s="15">
+        <f t="shared" si="4"/>
         <v>1354</v>
       </c>
-      <c r="J63" t="str">
-        <f>"\u"&amp;TEXT(I63,"0000")&amp;"?"</f>
+      <c r="K63" t="str">
+        <f t="shared" si="5"/>
         <v>\u1354?</v>
       </c>
-      <c r="K63" t="s">
+      <c r="L63" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="19.5">
+    <row r="64" spans="1:12" ht="19.5">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5567,32 +5803,35 @@
         <v>61</v>
       </c>
       <c r="E64" s="24" t="str">
-        <f>F64</f>
+        <f t="shared" si="6"/>
         <v>å</v>
       </c>
       <c r="F64" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D64,2)))</f>
+        <f t="shared" si="7"/>
         <v>å</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="H64" s="16" t="s">
+      <c r="H64" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="I64" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="I64" s="15">
-        <f>HEX2DEC(H64)</f>
+      <c r="J64" s="15">
+        <f t="shared" si="4"/>
         <v>1402</v>
       </c>
-      <c r="J64" t="str">
-        <f>"\u"&amp;TEXT(I64,"0000")&amp;"?"</f>
+      <c r="K64" t="str">
+        <f t="shared" si="5"/>
         <v>\u1402?</v>
       </c>
-      <c r="K64" t="s">
+      <c r="L64" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="19.5">
+    <row r="65" spans="1:12" ht="19.5">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5606,32 +5845,35 @@
         <v>62</v>
       </c>
       <c r="E65" s="24" t="str">
-        <f>F65</f>
+        <f t="shared" si="6"/>
         <v>æ</v>
       </c>
       <c r="F65" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D65,2)))</f>
+        <f t="shared" si="7"/>
         <v>æ</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="H65" s="16" t="s">
+      <c r="H65" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="I65" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="I65" s="15">
-        <f>HEX2DEC(H65)</f>
+      <c r="J65" s="15">
+        <f t="shared" si="4"/>
         <v>1355</v>
       </c>
-      <c r="J65" t="str">
-        <f>"\u"&amp;TEXT(I65,"0000")&amp;"?"</f>
+      <c r="K65" t="str">
+        <f t="shared" si="5"/>
         <v>\u1355?</v>
       </c>
-      <c r="K65" t="s">
+      <c r="L65" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="19.5">
+    <row r="66" spans="1:12" ht="19.5">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5645,32 +5887,35 @@
         <v>63</v>
       </c>
       <c r="E66" s="24" t="str">
-        <f>F66</f>
+        <f t="shared" si="6"/>
         <v>ç</v>
       </c>
       <c r="F66" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D66,2)))</f>
+        <f t="shared" si="7"/>
         <v>ç</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="H66" s="16" t="s">
+      <c r="H66" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="I66" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="I66" s="15">
-        <f>HEX2DEC(H66)</f>
+      <c r="J66" s="15">
+        <f t="shared" ref="J66:J97" si="8">HEX2DEC(I66)</f>
         <v>1403</v>
       </c>
-      <c r="J66" t="str">
-        <f>"\u"&amp;TEXT(I66,"0000")&amp;"?"</f>
+      <c r="K66" t="str">
+        <f t="shared" ref="K66:K97" si="9">"\u"&amp;TEXT(J66,"0000")&amp;"?"</f>
         <v>\u1403?</v>
       </c>
-      <c r="K66" t="s">
+      <c r="L66" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="19.5">
+    <row r="67" spans="1:12" ht="19.5">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5684,32 +5929,35 @@
         <v>64</v>
       </c>
       <c r="E67" s="24" t="str">
-        <f>F67</f>
+        <f t="shared" ref="E67:E98" si="10">F67</f>
         <v>è</v>
       </c>
       <c r="F67" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D67,2)))</f>
+        <f t="shared" ref="F67:F89" si="11">CHAR(HEX2DEC(RIGHT(D67,2)))</f>
         <v>è</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="H67" s="16" t="s">
+      <c r="H67" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="I67" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="I67" s="15">
-        <f>HEX2DEC(H67)</f>
+      <c r="J67" s="15">
+        <f t="shared" si="8"/>
         <v>1356</v>
       </c>
-      <c r="J67" t="str">
-        <f>"\u"&amp;TEXT(I67,"0000")&amp;"?"</f>
+      <c r="K67" t="str">
+        <f t="shared" si="9"/>
         <v>\u1356?</v>
       </c>
-      <c r="K67" t="s">
+      <c r="L67" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="19.5">
+    <row r="68" spans="1:12" ht="19.5">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5723,32 +5971,35 @@
         <v>65</v>
       </c>
       <c r="E68" s="24" t="str">
-        <f>F68</f>
+        <f t="shared" si="10"/>
         <v>é</v>
       </c>
       <c r="F68" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D68,2)))</f>
+        <f t="shared" si="11"/>
         <v>é</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="H68" s="16" t="s">
+      <c r="H68" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="I68" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="I68" s="15">
-        <f>HEX2DEC(H68)</f>
+      <c r="J68" s="15">
+        <f t="shared" si="8"/>
         <v>1404</v>
       </c>
-      <c r="J68" t="str">
-        <f>"\u"&amp;TEXT(I68,"0000")&amp;"?"</f>
+      <c r="K68" t="str">
+        <f t="shared" si="9"/>
         <v>\u1404?</v>
       </c>
-      <c r="K68" t="s">
+      <c r="L68" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="19.5">
+    <row r="69" spans="1:12" ht="19.5">
       <c r="A69">
         <v>68</v>
       </c>
@@ -5762,32 +6013,35 @@
         <v>66</v>
       </c>
       <c r="E69" s="24" t="str">
-        <f>F69</f>
+        <f t="shared" si="10"/>
         <v>ê</v>
       </c>
       <c r="F69" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D69,2)))</f>
+        <f t="shared" si="11"/>
         <v>ê</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="H69" s="16" t="s">
+      <c r="H69" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="I69" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="I69" s="15">
-        <f>HEX2DEC(H69)</f>
+      <c r="J69" s="15">
+        <f t="shared" si="8"/>
         <v>1357</v>
       </c>
-      <c r="J69" t="str">
-        <f>"\u"&amp;TEXT(I69,"0000")&amp;"?"</f>
+      <c r="K69" t="str">
+        <f t="shared" si="9"/>
         <v>\u1357?</v>
       </c>
-      <c r="K69" t="s">
+      <c r="L69" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="19.5">
+    <row r="70" spans="1:12" ht="19.5">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5801,32 +6055,35 @@
         <v>67</v>
       </c>
       <c r="E70" s="24" t="str">
-        <f>F70</f>
+        <f t="shared" si="10"/>
         <v>ë</v>
       </c>
       <c r="F70" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D70,2)))</f>
+        <f t="shared" si="11"/>
         <v>ë</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="H70" s="16" t="s">
+      <c r="H70" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="I70" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="I70" s="15">
-        <f>HEX2DEC(H70)</f>
+      <c r="J70" s="15">
+        <f t="shared" si="8"/>
         <v>1405</v>
       </c>
-      <c r="J70" t="str">
-        <f>"\u"&amp;TEXT(I70,"0000")&amp;"?"</f>
+      <c r="K70" t="str">
+        <f t="shared" si="9"/>
         <v>\u1405?</v>
       </c>
-      <c r="K70" t="s">
+      <c r="L70" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="19.5">
+    <row r="71" spans="1:12" ht="19.5">
       <c r="A71">
         <v>70</v>
       </c>
@@ -5840,32 +6097,35 @@
         <v>68</v>
       </c>
       <c r="E71" s="24" t="str">
-        <f>F71</f>
+        <f t="shared" si="10"/>
         <v>ì</v>
       </c>
       <c r="F71" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D71,2)))</f>
+        <f t="shared" si="11"/>
         <v>ì</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="H71" s="16" t="s">
+      <c r="H71" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="I71" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="I71" s="15">
-        <f>HEX2DEC(H71)</f>
+      <c r="J71" s="15">
+        <f t="shared" si="8"/>
         <v>1358</v>
       </c>
-      <c r="J71" t="str">
-        <f>"\u"&amp;TEXT(I71,"0000")&amp;"?"</f>
+      <c r="K71" t="str">
+        <f t="shared" si="9"/>
         <v>\u1358?</v>
       </c>
-      <c r="K71" t="s">
+      <c r="L71" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="19.5">
+    <row r="72" spans="1:12" ht="19.5">
       <c r="A72">
         <v>71</v>
       </c>
@@ -5879,32 +6139,35 @@
         <v>69</v>
       </c>
       <c r="E72" s="24" t="str">
-        <f>F72</f>
+        <f t="shared" si="10"/>
         <v>í</v>
       </c>
       <c r="F72" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D72,2)))</f>
+        <f t="shared" si="11"/>
         <v>í</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="H72" s="16" t="s">
+      <c r="H72" s="31" t="s">
+        <v>275</v>
+      </c>
+      <c r="I72" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="I72" s="15">
-        <f>HEX2DEC(H72)</f>
+      <c r="J72" s="15">
+        <f t="shared" si="8"/>
         <v>1406</v>
       </c>
-      <c r="J72" t="str">
-        <f>"\u"&amp;TEXT(I72,"0000")&amp;"?"</f>
+      <c r="K72" t="str">
+        <f t="shared" si="9"/>
         <v>\u1406?</v>
       </c>
-      <c r="K72" t="s">
+      <c r="L72" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="19.5">
+    <row r="73" spans="1:12" ht="19.5">
       <c r="A73">
         <v>72</v>
       </c>
@@ -5918,32 +6181,35 @@
         <v>70</v>
       </c>
       <c r="E73" s="24" t="str">
-        <f>F73</f>
+        <f t="shared" si="10"/>
         <v>î</v>
       </c>
       <c r="F73" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D73,2)))</f>
+        <f t="shared" si="11"/>
         <v>î</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="H73" s="16" t="s">
+      <c r="H73" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="I73" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="I73" s="15">
-        <f>HEX2DEC(H73)</f>
+      <c r="J73" s="15">
+        <f t="shared" si="8"/>
         <v>1359</v>
       </c>
-      <c r="J73" t="str">
-        <f>"\u"&amp;TEXT(I73,"0000")&amp;"?"</f>
+      <c r="K73" t="str">
+        <f t="shared" si="9"/>
         <v>\u1359?</v>
       </c>
-      <c r="K73" t="s">
+      <c r="L73" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="19.5">
+    <row r="74" spans="1:12" ht="19.5">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5957,32 +6223,35 @@
         <v>71</v>
       </c>
       <c r="E74" s="24" t="str">
-        <f>F74</f>
+        <f t="shared" si="10"/>
         <v>ï</v>
       </c>
       <c r="F74" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D74,2)))</f>
+        <f t="shared" si="11"/>
         <v>ï</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="H74" s="16" t="s">
+      <c r="H74" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="I74" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="I74" s="15">
-        <f>HEX2DEC(H74)</f>
+      <c r="J74" s="15">
+        <f t="shared" si="8"/>
         <v>1407</v>
       </c>
-      <c r="J74" t="str">
-        <f>"\u"&amp;TEXT(I74,"0000")&amp;"?"</f>
+      <c r="K74" t="str">
+        <f t="shared" si="9"/>
         <v>\u1407?</v>
       </c>
-      <c r="K74" t="s">
+      <c r="L74" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="19.5">
+    <row r="75" spans="1:12" ht="19.5">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5996,32 +6265,35 @@
         <v>72</v>
       </c>
       <c r="E75" s="24" t="str">
-        <f>F75</f>
+        <f t="shared" si="10"/>
         <v>ð</v>
       </c>
       <c r="F75" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D75,2)))</f>
+        <f t="shared" si="11"/>
         <v>ð</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="H75" s="16" t="s">
+      <c r="H75" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="I75" s="16" t="s">
         <v>350</v>
       </c>
-      <c r="I75" s="15">
-        <f>HEX2DEC(H75)</f>
+      <c r="J75" s="15">
+        <f t="shared" si="8"/>
         <v>1360</v>
       </c>
-      <c r="J75" t="str">
-        <f>"\u"&amp;TEXT(I75,"0000")&amp;"?"</f>
+      <c r="K75" t="str">
+        <f t="shared" si="9"/>
         <v>\u1360?</v>
       </c>
-      <c r="K75" t="s">
+      <c r="L75" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="19.5">
+    <row r="76" spans="1:12" ht="19.5">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6035,32 +6307,35 @@
         <v>73</v>
       </c>
       <c r="E76" s="24" t="str">
-        <f>F76</f>
+        <f t="shared" si="10"/>
         <v>ñ</v>
       </c>
       <c r="F76" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D76,2)))</f>
+        <f t="shared" si="11"/>
         <v>ñ</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="H76" s="16" t="s">
+      <c r="H76" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="I76" s="16" t="s">
         <v>351</v>
       </c>
-      <c r="I76" s="15">
-        <f>HEX2DEC(H76)</f>
+      <c r="J76" s="15">
+        <f t="shared" si="8"/>
         <v>1408</v>
       </c>
-      <c r="J76" t="str">
-        <f>"\u"&amp;TEXT(I76,"0000")&amp;"?"</f>
+      <c r="K76" t="str">
+        <f t="shared" si="9"/>
         <v>\u1408?</v>
       </c>
-      <c r="K76" t="s">
+      <c r="L76" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="19.5">
+    <row r="77" spans="1:12" ht="19.5">
       <c r="A77">
         <v>76</v>
       </c>
@@ -6074,32 +6349,35 @@
         <v>74</v>
       </c>
       <c r="E77" s="24" t="str">
-        <f>F77</f>
+        <f t="shared" si="10"/>
         <v>ò</v>
       </c>
       <c r="F77" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D77,2)))</f>
+        <f t="shared" si="11"/>
         <v>ò</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="H77" s="16" t="s">
+      <c r="H77" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="I77" s="16" t="s">
         <v>352</v>
       </c>
-      <c r="I77" s="15">
-        <f>HEX2DEC(H77)</f>
+      <c r="J77" s="15">
+        <f t="shared" si="8"/>
         <v>1361</v>
       </c>
-      <c r="J77" t="str">
-        <f>"\u"&amp;TEXT(I77,"0000")&amp;"?"</f>
+      <c r="K77" t="str">
+        <f t="shared" si="9"/>
         <v>\u1361?</v>
       </c>
-      <c r="K77" t="s">
+      <c r="L77" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="19.5">
+    <row r="78" spans="1:12" ht="19.5">
       <c r="A78">
         <v>77</v>
       </c>
@@ -6113,32 +6391,35 @@
         <v>75</v>
       </c>
       <c r="E78" s="24" t="str">
-        <f>F78</f>
+        <f t="shared" si="10"/>
         <v>ó</v>
       </c>
       <c r="F78" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D78,2)))</f>
+        <f t="shared" si="11"/>
         <v>ó</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="H78" s="16" t="s">
+      <c r="H78" s="31" t="s">
+        <v>282</v>
+      </c>
+      <c r="I78" s="16" t="s">
         <v>353</v>
       </c>
-      <c r="I78" s="15">
-        <f>HEX2DEC(H78)</f>
+      <c r="J78" s="15">
+        <f t="shared" si="8"/>
         <v>1409</v>
       </c>
-      <c r="J78" t="str">
-        <f>"\u"&amp;TEXT(I78,"0000")&amp;"?"</f>
+      <c r="K78" t="str">
+        <f t="shared" si="9"/>
         <v>\u1409?</v>
       </c>
-      <c r="K78" t="s">
+      <c r="L78" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="19.5">
+    <row r="79" spans="1:12" ht="19.5">
       <c r="A79">
         <v>78</v>
       </c>
@@ -6152,32 +6433,35 @@
         <v>76</v>
       </c>
       <c r="E79" s="24" t="str">
-        <f>F79</f>
+        <f t="shared" si="10"/>
         <v>ô</v>
       </c>
       <c r="F79" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D79,2)))</f>
+        <f t="shared" si="11"/>
         <v>ô</v>
       </c>
       <c r="G79" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="H79" s="16" t="s">
+      <c r="H79" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="I79" s="16" t="s">
         <v>354</v>
       </c>
-      <c r="I79" s="15">
-        <f>HEX2DEC(H79)</f>
+      <c r="J79" s="15">
+        <f t="shared" si="8"/>
         <v>1362</v>
       </c>
-      <c r="J79" t="str">
-        <f>"\u"&amp;TEXT(I79,"0000")&amp;"?"</f>
+      <c r="K79" t="str">
+        <f t="shared" si="9"/>
         <v>\u1362?</v>
       </c>
-      <c r="K79" t="s">
+      <c r="L79" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="19.5">
+    <row r="80" spans="1:12" ht="19.5">
       <c r="A80">
         <v>79</v>
       </c>
@@ -6191,32 +6475,35 @@
         <v>77</v>
       </c>
       <c r="E80" s="24" t="str">
-        <f>F80</f>
+        <f t="shared" si="10"/>
         <v>õ</v>
       </c>
       <c r="F80" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D80,2)))</f>
+        <f t="shared" si="11"/>
         <v>õ</v>
       </c>
       <c r="G80" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="H80" s="16" t="s">
+      <c r="H80" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="I80" s="16" t="s">
         <v>355</v>
       </c>
-      <c r="I80" s="15">
-        <f>HEX2DEC(H80)</f>
+      <c r="J80" s="15">
+        <f t="shared" si="8"/>
         <v>1410</v>
       </c>
-      <c r="J80" t="str">
-        <f>"\u"&amp;TEXT(I80,"0000")&amp;"?"</f>
+      <c r="K80" t="str">
+        <f t="shared" si="9"/>
         <v>\u1410?</v>
       </c>
-      <c r="K80" t="s">
+      <c r="L80" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="19.5">
+    <row r="81" spans="1:13" ht="19.5">
       <c r="A81">
         <v>80</v>
       </c>
@@ -6230,32 +6517,35 @@
         <v>78</v>
       </c>
       <c r="E81" s="24" t="str">
-        <f>F81</f>
+        <f t="shared" si="10"/>
         <v>ö</v>
       </c>
       <c r="F81" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D81,2)))</f>
+        <f t="shared" si="11"/>
         <v>ö</v>
       </c>
       <c r="G81" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="H81" s="16" t="s">
+      <c r="H81" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="I81" s="16" t="s">
         <v>356</v>
       </c>
-      <c r="I81" s="15">
-        <f>HEX2DEC(H81)</f>
+      <c r="J81" s="15">
+        <f t="shared" si="8"/>
         <v>1363</v>
       </c>
-      <c r="J81" t="str">
-        <f>"\u"&amp;TEXT(I81,"0000")&amp;"?"</f>
+      <c r="K81" t="str">
+        <f t="shared" si="9"/>
         <v>\u1363?</v>
       </c>
-      <c r="K81" t="s">
+      <c r="L81" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="19.5">
+    <row r="82" spans="1:13" ht="19.5">
       <c r="A82">
         <v>81</v>
       </c>
@@ -6269,32 +6559,35 @@
         <v>79</v>
       </c>
       <c r="E82" s="24" t="str">
-        <f>F82</f>
+        <f t="shared" si="10"/>
         <v>÷</v>
       </c>
       <c r="F82" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D82,2)))</f>
+        <f t="shared" si="11"/>
         <v>÷</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="H82" s="16" t="s">
+      <c r="H82" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="I82" s="16" t="s">
         <v>357</v>
       </c>
-      <c r="I82" s="15">
-        <f>HEX2DEC(H82)</f>
+      <c r="J82" s="15">
+        <f t="shared" si="8"/>
         <v>1411</v>
       </c>
-      <c r="J82" t="str">
-        <f>"\u"&amp;TEXT(I82,"0000")&amp;"?"</f>
+      <c r="K82" t="str">
+        <f t="shared" si="9"/>
         <v>\u1411?</v>
       </c>
-      <c r="K82" t="s">
+      <c r="L82" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="19.5">
+    <row r="83" spans="1:13" ht="19.5">
       <c r="A83">
         <v>82</v>
       </c>
@@ -6308,32 +6601,35 @@
         <v>80</v>
       </c>
       <c r="E83" s="24" t="str">
-        <f>F83</f>
+        <f t="shared" si="10"/>
         <v>ø</v>
       </c>
       <c r="F83" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D83,2)))</f>
+        <f t="shared" si="11"/>
         <v>ø</v>
       </c>
       <c r="G83" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="H83" s="16" t="s">
+      <c r="H83" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="I83" s="16" t="s">
         <v>358</v>
       </c>
-      <c r="I83" s="15">
-        <f>HEX2DEC(H83)</f>
+      <c r="J83" s="15">
+        <f t="shared" si="8"/>
         <v>1364</v>
       </c>
-      <c r="J83" t="str">
-        <f>"\u"&amp;TEXT(I83,"0000")&amp;"?"</f>
+      <c r="K83" t="str">
+        <f t="shared" si="9"/>
         <v>\u1364?</v>
       </c>
-      <c r="K83" t="s">
+      <c r="L83" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="19.5">
+    <row r="84" spans="1:13" ht="19.5">
       <c r="A84">
         <v>83</v>
       </c>
@@ -6347,32 +6643,35 @@
         <v>81</v>
       </c>
       <c r="E84" s="24" t="str">
-        <f>F84</f>
+        <f t="shared" si="10"/>
         <v>ù</v>
       </c>
       <c r="F84" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D84,2)))</f>
+        <f t="shared" si="11"/>
         <v>ù</v>
       </c>
       <c r="G84" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="H84" s="16" t="s">
+      <c r="H84" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="I84" s="16" t="s">
         <v>359</v>
       </c>
-      <c r="I84" s="15">
-        <f>HEX2DEC(H84)</f>
+      <c r="J84" s="15">
+        <f t="shared" si="8"/>
         <v>1412</v>
       </c>
-      <c r="J84" t="str">
-        <f>"\u"&amp;TEXT(I84,"0000")&amp;"?"</f>
+      <c r="K84" t="str">
+        <f t="shared" si="9"/>
         <v>\u1412?</v>
       </c>
-      <c r="K84" t="s">
+      <c r="L84" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="19.5">
+    <row r="85" spans="1:13" ht="19.5">
       <c r="A85">
         <v>84</v>
       </c>
@@ -6386,32 +6685,35 @@
         <v>82</v>
       </c>
       <c r="E85" s="24" t="str">
-        <f>F85</f>
+        <f t="shared" si="10"/>
         <v>ú</v>
       </c>
       <c r="F85" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D85,2)))</f>
+        <f t="shared" si="11"/>
         <v>ú</v>
       </c>
       <c r="G85" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="H85" s="16" t="s">
+      <c r="H85" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="I85" s="16" t="s">
         <v>360</v>
       </c>
-      <c r="I85" s="15">
-        <f>HEX2DEC(H85)</f>
+      <c r="J85" s="15">
+        <f t="shared" si="8"/>
         <v>1365</v>
       </c>
-      <c r="J85" t="str">
-        <f>"\u"&amp;TEXT(I85,"0000")&amp;"?"</f>
+      <c r="K85" t="str">
+        <f t="shared" si="9"/>
         <v>\u1365?</v>
       </c>
-      <c r="K85" t="s">
+      <c r="L85" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="19.5">
+    <row r="86" spans="1:13" ht="19.5">
       <c r="A86">
         <v>85</v>
       </c>
@@ -6425,32 +6727,35 @@
         <v>83</v>
       </c>
       <c r="E86" s="24" t="str">
-        <f>F86</f>
+        <f t="shared" si="10"/>
         <v>û</v>
       </c>
       <c r="F86" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D86,2)))</f>
+        <f t="shared" si="11"/>
         <v>û</v>
       </c>
       <c r="G86" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="H86" s="16" t="s">
+      <c r="H86" s="31" t="s">
+        <v>290</v>
+      </c>
+      <c r="I86" s="16" t="s">
         <v>361</v>
       </c>
-      <c r="I86" s="15">
-        <f>HEX2DEC(H86)</f>
+      <c r="J86" s="15">
+        <f t="shared" si="8"/>
         <v>1413</v>
       </c>
-      <c r="J86" t="str">
-        <f>"\u"&amp;TEXT(I86,"0000")&amp;"?"</f>
+      <c r="K86" t="str">
+        <f t="shared" si="9"/>
         <v>\u1413?</v>
       </c>
-      <c r="K86" t="s">
+      <c r="L86" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="19.5">
+    <row r="87" spans="1:13" ht="19.5">
       <c r="A87">
         <v>86</v>
       </c>
@@ -6464,32 +6769,35 @@
         <v>84</v>
       </c>
       <c r="E87" s="24" t="str">
-        <f>F87</f>
+        <f t="shared" si="10"/>
         <v>ü</v>
       </c>
       <c r="F87" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D87,2)))</f>
+        <f t="shared" si="11"/>
         <v>ü</v>
       </c>
       <c r="G87" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="H87" s="16" t="s">
+      <c r="H87" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="I87" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="I87" s="15">
-        <f>HEX2DEC(H87)</f>
+      <c r="J87" s="15">
+        <f t="shared" si="8"/>
         <v>1366</v>
       </c>
-      <c r="J87" t="str">
-        <f>"\u"&amp;TEXT(I87,"0000")&amp;"?"</f>
+      <c r="K87" t="str">
+        <f t="shared" si="9"/>
         <v>\u1366?</v>
       </c>
-      <c r="K87" t="s">
+      <c r="L87" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="19.5">
+    <row r="88" spans="1:13" ht="19.5">
       <c r="A88">
         <v>87</v>
       </c>
@@ -6503,32 +6811,35 @@
         <v>85</v>
       </c>
       <c r="E88" s="24" t="str">
-        <f>F88</f>
+        <f t="shared" si="10"/>
         <v>ý</v>
       </c>
       <c r="F88" s="7" t="str">
-        <f>CHAR(HEX2DEC(RIGHT(D88,2)))</f>
+        <f t="shared" si="11"/>
         <v>ý</v>
       </c>
       <c r="G88" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="H88" s="16" t="s">
+      <c r="H88" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="I88" s="16" t="s">
         <v>363</v>
       </c>
-      <c r="I88" s="15">
-        <f>HEX2DEC(H88)</f>
+      <c r="J88" s="15">
+        <f t="shared" si="8"/>
         <v>1414</v>
       </c>
-      <c r="J88" t="str">
-        <f>"\u"&amp;TEXT(I88,"0000")&amp;"?"</f>
+      <c r="K88" t="str">
+        <f t="shared" si="9"/>
         <v>\u1414?</v>
       </c>
-      <c r="K88" t="s">
+      <c r="L88" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="19.5">
+    <row r="89" spans="1:13" ht="19.5">
       <c r="A89">
         <v>88</v>
       </c>
@@ -6544,25 +6855,28 @@
       <c r="G89" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="H89" s="16" t="s">
+      <c r="H89" s="31" t="s">
+        <v>295</v>
+      </c>
+      <c r="I89" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="I89" s="15">
-        <f>HEX2DEC(H89)</f>
+      <c r="J89" s="15">
+        <f t="shared" si="8"/>
         <v>1418</v>
       </c>
-      <c r="J89" t="str">
-        <f>"\u"&amp;TEXT(I89,"0000")&amp;"?"</f>
+      <c r="K89" t="str">
+        <f t="shared" si="9"/>
         <v>\u1418?</v>
       </c>
-      <c r="K89" t="s">
+      <c r="L89" t="s">
         <v>296</v>
       </c>
-      <c r="L89" s="25" t="s">
+      <c r="M89" s="25" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="19.5">
+    <row r="90" spans="1:13" ht="19.5">
       <c r="A90">
         <v>89</v>
       </c>
@@ -6578,25 +6892,28 @@
       <c r="G90" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="H90" s="16" t="s">
+      <c r="H90" s="31" t="s">
+        <v>594</v>
+      </c>
+      <c r="I90" s="16" t="s">
         <v>591</v>
       </c>
-      <c r="I90" s="15">
-        <f>HEX2DEC(H90)</f>
+      <c r="J90" s="15">
+        <f t="shared" si="8"/>
         <v>1375</v>
       </c>
-      <c r="J90" t="str">
-        <f>"\u"&amp;TEXT(I90,"0000")&amp;"?"</f>
+      <c r="K90" t="str">
+        <f t="shared" si="9"/>
         <v>\u1375?</v>
       </c>
-      <c r="K90" t="s">
+      <c r="L90" t="s">
         <v>592</v>
       </c>
-      <c r="L90" s="25" t="s">
+      <c r="M90" s="25" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="19.5">
+    <row r="91" spans="1:13" ht="19.5">
       <c r="A91">
         <v>90</v>
       </c>
@@ -6612,25 +6929,28 @@
       <c r="G91" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="H91" s="16" t="s">
+      <c r="H91" s="31" t="s">
+        <v>590</v>
+      </c>
+      <c r="I91" s="16" t="s">
         <v>563</v>
       </c>
-      <c r="I91" s="15">
-        <f>HEX2DEC(H91)</f>
+      <c r="J91" s="15">
+        <f t="shared" si="8"/>
         <v>1423</v>
       </c>
-      <c r="J91" t="str">
-        <f>"\u"&amp;TEXT(I91,"0000")&amp;"?"</f>
+      <c r="K91" t="str">
+        <f t="shared" si="9"/>
         <v>\u1423?</v>
       </c>
-      <c r="K91" t="s">
+      <c r="L91" t="s">
         <v>562</v>
       </c>
-      <c r="L91" s="25" t="s">
+      <c r="M91" s="25" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="19.5">
+    <row r="92" spans="1:13" ht="19.5">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6646,22 +6966,25 @@
       <c r="G92" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="H92" s="17" t="s">
+      <c r="H92" s="31" t="s">
+        <v>577</v>
+      </c>
+      <c r="I92" s="17" t="s">
         <v>578</v>
       </c>
-      <c r="I92" s="15">
-        <f>HEX2DEC(H92)</f>
+      <c r="J92" s="15">
+        <f t="shared" si="8"/>
         <v>64275</v>
       </c>
-      <c r="J92" t="str">
-        <f>"\u"&amp;TEXT(I92,"0000")&amp;"?"</f>
+      <c r="K92" t="str">
+        <f t="shared" si="9"/>
         <v>\u64275?</v>
       </c>
-      <c r="K92" t="s">
+      <c r="L92" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="19.5">
+    <row r="93" spans="1:13" ht="19.5">
       <c r="A93">
         <v>92</v>
       </c>
@@ -6677,22 +7000,25 @@
       <c r="G93" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="H93" s="17" t="s">
+      <c r="H93" s="31" t="s">
+        <v>586</v>
+      </c>
+      <c r="I93" s="17" t="s">
         <v>579</v>
       </c>
-      <c r="I93" s="15">
-        <f>HEX2DEC(H93)</f>
+      <c r="J93" s="15">
+        <f t="shared" si="8"/>
         <v>64276</v>
       </c>
-      <c r="J93" t="str">
-        <f>"\u"&amp;TEXT(I93,"0000")&amp;"?"</f>
+      <c r="K93" t="str">
+        <f t="shared" si="9"/>
         <v>\u64276?</v>
       </c>
-      <c r="K93" t="s">
+      <c r="L93" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="19.5">
+    <row r="94" spans="1:13" ht="19.5">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6708,22 +7034,25 @@
       <c r="G94" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="H94" s="17" t="s">
+      <c r="H94" s="31" t="s">
+        <v>587</v>
+      </c>
+      <c r="I94" s="17" t="s">
         <v>580</v>
       </c>
-      <c r="I94" s="15">
-        <f>HEX2DEC(H94)</f>
+      <c r="J94" s="15">
+        <f t="shared" si="8"/>
         <v>64277</v>
       </c>
-      <c r="J94" t="str">
-        <f>"\u"&amp;TEXT(I94,"0000")&amp;"?"</f>
+      <c r="K94" t="str">
+        <f t="shared" si="9"/>
         <v>\u64277?</v>
       </c>
-      <c r="K94" t="s">
+      <c r="L94" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="19.5">
+    <row r="95" spans="1:13" ht="19.5">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6739,22 +7068,25 @@
       <c r="G95" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="H95" s="17" t="s">
+      <c r="H95" s="31" t="s">
+        <v>588</v>
+      </c>
+      <c r="I95" s="17" t="s">
         <v>581</v>
       </c>
-      <c r="I95" s="15">
-        <f>HEX2DEC(H95)</f>
+      <c r="J95" s="15">
+        <f t="shared" si="8"/>
         <v>64278</v>
       </c>
-      <c r="J95" t="str">
-        <f>"\u"&amp;TEXT(I95,"0000")&amp;"?"</f>
+      <c r="K95" t="str">
+        <f t="shared" si="9"/>
         <v>\u64278?</v>
       </c>
-      <c r="K95" t="s">
+      <c r="L95" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="19.5">
+    <row r="96" spans="1:13" ht="19.5">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6770,27 +7102,33 @@
       <c r="G96" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="H96" s="17" t="s">
+      <c r="H96" s="31" t="s">
+        <v>589</v>
+      </c>
+      <c r="I96" s="17" t="s">
         <v>582</v>
       </c>
-      <c r="I96" s="15">
-        <f>HEX2DEC(H96)</f>
+      <c r="J96" s="15">
+        <f t="shared" si="8"/>
         <v>64279</v>
       </c>
-      <c r="J96" t="str">
-        <f>"\u"&amp;TEXT(I96,"0000")&amp;"?"</f>
+      <c r="K96" t="str">
+        <f t="shared" si="9"/>
         <v>\u64279?</v>
       </c>
-      <c r="K96" t="s">
+      <c r="L96" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="98" spans="7:7" ht="19.5">
+    <row r="98" spans="7:8" ht="19.5">
       <c r="G98" s="3"/>
+      <c r="H98" s="31"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" autoFilter="0"/>
-  <autoFilter ref="A1:L96"/>
+  <autoFilter ref="A1:M96">
+    <filterColumn colId="7"/>
+  </autoFilter>
   <sortState ref="A2:L96">
     <sortCondition ref="A1"/>
   </sortState>

</xml_diff>